<commit_message>
Petits modifs Dictionnaire de données BDD 'utilisateurs' et 'filtres'
</commit_message>
<xml_diff>
--- a/textes/Dictionnaire_données.xlsx
+++ b/textes/Dictionnaire_données.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UTILISATEURS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="84">
   <si>
     <t>CODE</t>
   </si>
@@ -314,6 +314,27 @@
   </si>
   <si>
     <t>Pseudo du signalé</t>
+  </si>
+  <si>
+    <t>CODERECENT</t>
+  </si>
+  <si>
+    <t>CODEPOP</t>
+  </si>
+  <si>
+    <t>Récent</t>
+  </si>
+  <si>
+    <t>Populaire</t>
+  </si>
+  <si>
+    <t>Le voyage posté le plus récemment</t>
+  </si>
+  <si>
+    <t>Le voyage le plus liké/commenté</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY / Est relié à "voyages" = "titre"</t>
   </si>
 </sst>
 </file>
@@ -1378,20 +1399,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="3" max="3" width="37" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="5" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="71.28515625" customWidth="1"/>
+    <col min="7" max="7" width="69.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1478,26 +1499,26 @@
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="16">
         <v>60</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="16" t="s">
         <v>51</v>
       </c>
       <c r="H4" s="14"/>
@@ -1507,27 +1528,51 @@
       <c r="L4" s="14"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
+      <c r="A5" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>83</v>
+      </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
@@ -1591,13 +1636,13 @@
       <c r="L10" s="14"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -1605,13 +1650,13 @@
       <c r="L11" s="14"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
@@ -1771,6 +1816,34 @@
       <c r="J23" s="14"/>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2580,7 +2653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modifs Dictionnaire de données
</commit_message>
<xml_diff>
--- a/textes/Dictionnaire_données.xlsx
+++ b/textes/Dictionnaire_données.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmes\Xampp\htdocs\TRAVELOG\textes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoan\Documents\AFPA Développeur Web\Projet fil rouge\projet\textes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C82D598-AB41-4346-A4BD-6194D9061170}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UTILISATEURS" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="87">
   <si>
     <t>CODE</t>
   </si>
@@ -128,9 +129,6 @@
   </si>
   <si>
     <t>nath</t>
-  </si>
-  <si>
-    <t>yoann</t>
   </si>
   <si>
     <t>NULL</t>
@@ -336,11 +334,23 @@
   <si>
     <t>FOREIGN KEY / Est relié à "voyages" = "titre"</t>
   </si>
+  <si>
+    <t>USERFRIEND</t>
+  </si>
+  <si>
+    <t>yoan</t>
+  </si>
+  <si>
+    <t>USERREPORT</t>
+  </si>
+  <si>
+    <t>USERREPORTED</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -940,7 +950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -971,10 +981,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G1" s="14"/>
       <c r="H1" s="14"/>
@@ -987,14 +997,14 @@
         <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>19</v>
@@ -1010,7 +1020,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>11</v>
@@ -1019,10 +1029,10 @@
         <v>20</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
@@ -1035,17 +1045,17 @@
         <v>22</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -1058,7 +1068,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>11</v>
@@ -1067,7 +1077,7 @@
         <v>50</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="14"/>
@@ -1081,7 +1091,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>11</v>
@@ -1090,7 +1100,7 @@
         <v>50</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="14"/>
@@ -1104,7 +1114,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>18</v>
@@ -1113,10 +1123,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -1129,7 +1139,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>11</v>
@@ -1138,7 +1148,7 @@
         <v>50</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="14"/>
@@ -1152,17 +1162,17 @@
         <v>27</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -1184,7 +1194,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>29</v>
@@ -1197,10 +1207,10 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>36</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>11</v>
@@ -1209,7 +1219,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>29</v>
@@ -1398,10 +1408,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1432,10 +1442,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
@@ -1460,10 +1470,10 @@
         <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -1488,10 +1498,10 @@
         <v>60</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -1516,10 +1526,10 @@
         <v>60</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
@@ -1529,23 +1539,23 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -1555,23 +1565,23 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
@@ -1851,7 +1861,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1883,10 +1893,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
@@ -1897,7 +1907,7 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2"/>
@@ -1913,7 +1923,7 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
@@ -1929,7 +1939,7 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="7"/>
@@ -1945,7 +1955,7 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="5"/>
@@ -1961,7 +1971,7 @@
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="7"/>
@@ -1977,7 +1987,7 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="5"/>
@@ -1993,14 +2003,14 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="3"/>
       <c r="G8" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -2011,7 +2021,7 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="5"/>
@@ -2027,7 +2037,7 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="7"/>
@@ -2043,7 +2053,7 @@
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="24"/>
       <c r="D11" s="22"/>
@@ -2058,7 +2068,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="18"/>
       <c r="E12" s="18"/>
@@ -2072,7 +2082,7 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="24"/>
       <c r="D13" s="22"/>
@@ -2092,7 +2102,7 @@
       <c r="C14" s="18"/>
       <c r="E14" s="18"/>
       <c r="G14" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
@@ -2110,7 +2120,7 @@
       <c r="E15" s="24"/>
       <c r="F15" s="22"/>
       <c r="G15" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -2128,7 +2138,7 @@
       <c r="E16" s="21"/>
       <c r="F16" s="19"/>
       <c r="G16" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
@@ -2194,17 +2204,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="6" width="19.85546875" customWidth="1"/>
     <col min="7" max="7" width="43.28515625" customWidth="1"/>
   </cols>
@@ -2226,10 +2238,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
@@ -2238,16 +2250,24 @@
       <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
+      <c r="A2" s="26" t="s">
+        <v>83</v>
+      </c>
       <c r="B2" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="28"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="D2" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="27">
+        <v>20</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>37</v>
+      </c>
       <c r="G2" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -2271,7 +2291,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -2411,7 +2431,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2443,10 +2463,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
@@ -2457,14 +2477,14 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
       <c r="G2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -2475,14 +2495,14 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="6"/>
       <c r="G3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -2493,14 +2513,14 @@
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="9"/>
       <c r="G4" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
@@ -2650,19 +2670,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="34.42578125" customWidth="1"/>
-    <col min="5" max="6" width="16.5703125" customWidth="1"/>
+    <col min="4" max="6" width="16.5703125" customWidth="1"/>
     <col min="7" max="7" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2683,10 +2703,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
@@ -2695,16 +2715,24 @@
       <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="G2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -2713,16 +2741,24 @@
       <c r="L2" s="14"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
+      <c r="A3" s="29" t="s">
+        <v>86</v>
+      </c>
       <c r="B3" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="9"/>
+      <c r="D3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="10">
+        <v>20</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="G3" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -2746,7 +2782,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>

</xml_diff>

<commit_message>
Ajout de la section Voyage dans le dictionnaire de données
</commit_message>
<xml_diff>
--- a/textes/Dictionnaire_données.xlsx
+++ b/textes/Dictionnaire_données.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoan\Documents\AFPA Développeur Web\Projet fil rouge\projet\textes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Fil_Rouge\pfrTravelog\textes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C82D598-AB41-4346-A4BD-6194D9061170}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="UTILISATEURS" sheetId="1" r:id="rId1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="116">
   <si>
     <t>CODE</t>
   </si>
@@ -263,9 +262,6 @@
     <t>Textes</t>
   </si>
   <si>
-    <t>Est rélié à "Filtres voyages"</t>
-  </si>
-  <si>
     <t>Pseudo ami</t>
   </si>
   <si>
@@ -346,11 +342,102 @@
   <si>
     <t>USERREPORTED</t>
   </si>
+  <si>
+    <t>TRIPTITLE</t>
+  </si>
+  <si>
+    <t>TRIPDESC</t>
+  </si>
+  <si>
+    <t>TRIPDEBUT</t>
+  </si>
+  <si>
+    <t>TRIPFIN</t>
+  </si>
+  <si>
+    <t>TRIPMEDIA</t>
+  </si>
+  <si>
+    <t>TRIPCOUVERTURE</t>
+  </si>
+  <si>
+    <t>TRIPSTATUT</t>
+  </si>
+  <si>
+    <t>TRIPVU</t>
+  </si>
+  <si>
+    <t>TRIPLIKE</t>
+  </si>
+  <si>
+    <t>TRIPCOMM</t>
+  </si>
+  <si>
+    <t>TRIPSSTITRE</t>
+  </si>
+  <si>
+    <t>TRIPTEXT</t>
+  </si>
+  <si>
+    <t>Continent du voyage</t>
+  </si>
+  <si>
+    <t>Pays du du voyage</t>
+  </si>
+  <si>
+    <t>Ville du voyage</t>
+  </si>
+  <si>
+    <t>Titre du voyage</t>
+  </si>
+  <si>
+    <t>Description du voyage</t>
+  </si>
+  <si>
+    <t>Nombre de vues du voyage</t>
+  </si>
+  <si>
+    <t>Nombre de likes du voyage</t>
+  </si>
+  <si>
+    <t>Date du début du voyage</t>
+  </si>
+  <si>
+    <t>Date de fin du voyage</t>
+  </si>
+  <si>
+    <t>Photos/Videos dans chaque étape</t>
+  </si>
+  <si>
+    <t>Photo de couverture du voyage</t>
+  </si>
+  <si>
+    <t>Commentaire de chaque étape du voyage</t>
+  </si>
+  <si>
+    <t>Sous-titre de chaque étape du voyage</t>
+  </si>
+  <si>
+    <t>Texte pour chaque étape du voyage</t>
+  </si>
+  <si>
+    <t>IMG/VIDEO</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>Les caractères spéciaux ne sont pas acceptés
+(hors lettres avec accents, ‘ç’, ‘-‘, ‘ ?’, ‘ !’ et ‘ :’)</t>
+  </si>
+  <si>
+    <t>Est relié à "Filtres voyages"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -596,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -645,17 +732,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -670,6 +752,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -950,11 +1044,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,11 +1502,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1539,13 +1633,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>11</v>
@@ -1555,7 +1649,7 @@
         <v>37</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -1565,13 +1659,13 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>11</v>
@@ -1581,7 +1675,7 @@
         <v>37</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
@@ -1861,19 +1955,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" customWidth="1"/>
-    <col min="5" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="46.28515625" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1904,32 +2001,56 @@
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="2"/>
+      <c r="C2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2">
+        <v>50</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>114</v>
+      </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
       <c r="L2" s="14"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="B3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="5"/>
+      <c r="C3" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2000</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>114</v>
+      </c>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
@@ -1937,15 +2058,27 @@
       <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="B4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="7"/>
+      <c r="C4" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="7">
+        <v>8</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
@@ -1953,15 +2086,27 @@
       <c r="L4" s="14"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="B5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="5"/>
+      <c r="C5" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
@@ -1969,14 +2114,22 @@
       <c r="L5" s="14"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="B6" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="7"/>
+      <c r="C6" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="E6" s="7"/>
-      <c r="F6" s="3"/>
+      <c r="F6" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
@@ -1985,14 +2138,22 @@
       <c r="L6" s="14"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="B7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="G7" s="5"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
@@ -2001,14 +2162,24 @@
       <c r="L7" s="14"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="B8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="3"/>
+      <c r="C8" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="7">
+        <v>6</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="G8" s="7" t="s">
         <v>59</v>
       </c>
@@ -2019,14 +2190,24 @@
       <c r="L8" s="14"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="A9" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="B9" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" s="5">
+        <v>12</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
@@ -2035,14 +2216,24 @@
       <c r="L9" s="14"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="B10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="7">
+        <v>12</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -2050,45 +2241,84 @@
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23" t="s">
+    <row r="11" spans="1:12" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="24"/>
+      <c r="C11" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="5">
+        <v>500</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>114</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="B12" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="C12" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="7">
+        <v>40</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>114</v>
+      </c>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23" t="s">
+    <row r="13" spans="1:12" ht="61.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="24"/>
+      <c r="C13" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="5">
+        <v>500</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>114</v>
+      </c>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
@@ -2096,13 +2326,26 @@
       <c r="L13" s="14"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="E14" s="18"/>
+      <c r="C14" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="7">
+        <v>20</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="G14" s="7" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
@@ -2111,16 +2354,26 @@
       <c r="L14" s="14"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23" t="s">
+      <c r="A15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="22"/>
+      <c r="C15" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="5">
+        <v>60</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="G15" s="5" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -2128,17 +2381,27 @@
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20" t="s">
+    <row r="16" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="25" t="s">
-        <v>65</v>
+      <c r="C16" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="20">
+        <v>60</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>115</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
@@ -2200,14 +2463,15 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -2250,24 +2514,24 @@
       <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="27" t="s">
+      <c r="A2" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="27">
+      <c r="E2" s="22">
         <v>20</v>
       </c>
-      <c r="F2" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>68</v>
+      <c r="F2" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>67</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -2291,7 +2555,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -2431,7 +2695,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2477,14 +2741,14 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
       <c r="G2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -2495,7 +2759,7 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
@@ -2513,14 +2777,14 @@
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="9"/>
       <c r="G4" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
@@ -2670,7 +2934,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2716,10 +2980,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2" t="s">
@@ -2732,7 +2996,7 @@
         <v>37</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -2741,11 +3005,11 @@
       <c r="L2" s="14"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
-        <v>86</v>
+      <c r="A3" s="24" t="s">
+        <v>85</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="10" t="s">
@@ -2758,7 +3022,7 @@
         <v>37</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -2782,7 +3046,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>

</xml_diff>

<commit_message>
modifications dictionnaire de données
</commit_message>
<xml_diff>
--- a/textes/Dictionnaire_données.xlsx
+++ b/textes/Dictionnaire_données.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Fil_Rouge\pfrTravelog\textes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pfrTravelog\textes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" activeTab="2"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="UTILISATEURS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="124">
   <si>
     <t>CODE</t>
   </si>
@@ -298,12 +298,6 @@
     <t>Demande d'ami</t>
   </si>
   <si>
-    <t>Est relié à "Voyages"</t>
-  </si>
-  <si>
-    <t>Est relié à "Amis"</t>
-  </si>
-  <si>
     <t>Pseudo du signalant</t>
   </si>
   <si>
@@ -432,6 +426,36 @@
   </si>
   <si>
     <t>Est relié à "Filtres voyages"</t>
+  </si>
+  <si>
+    <t>notifComm</t>
+  </si>
+  <si>
+    <t>notifLike</t>
+  </si>
+  <si>
+    <t>notifAmi</t>
+  </si>
+  <si>
+    <t>Notification de commentaire non lu</t>
+  </si>
+  <si>
+    <t>Badge rouge et qui est lié à "Voyages"</t>
+  </si>
+  <si>
+    <t>Notification de nouveau like</t>
+  </si>
+  <si>
+    <t>Notification de demande d'ami</t>
+  </si>
+  <si>
+    <t>Badge rouge et qui est lié aux "likes"</t>
+  </si>
+  <si>
+    <t>Badge rouge et qui est lié à "amis"</t>
+  </si>
+  <si>
+    <t>OUI</t>
   </si>
 </sst>
 </file>
@@ -683,7 +707,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -764,6 +788,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1048,7 +1075,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,13 +1660,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>77</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>79</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>11</v>
@@ -1649,7 +1676,7 @@
         <v>37</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -1659,13 +1686,13 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>11</v>
@@ -1675,7 +1702,7 @@
         <v>37</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
@@ -1958,7 +1985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -2003,13 +2030,13 @@
     </row>
     <row r="2" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
@@ -2021,7 +2048,7 @@
         <v>37</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -2031,13 +2058,13 @@
     </row>
     <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -2049,7 +2076,7 @@
         <v>37</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -2059,13 +2086,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>18</v>
@@ -2087,13 +2114,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>18</v>
@@ -2115,16 +2142,16 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="6" t="s">
@@ -2139,16 +2166,16 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="6" t="s">
@@ -2163,7 +2190,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>58</v>
@@ -2191,16 +2218,16 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E9" s="5">
         <v>12</v>
@@ -2217,16 +2244,16 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E10" s="7">
         <v>12</v>
@@ -2243,13 +2270,13 @@
     </row>
     <row r="11" spans="1:12" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>62</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>11</v>
@@ -2261,7 +2288,7 @@
         <v>37</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
@@ -2271,13 +2298,13 @@
     </row>
     <row r="12" spans="1:12" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>63</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>11</v>
@@ -2289,7 +2316,7 @@
         <v>37</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
@@ -2299,13 +2326,13 @@
     </row>
     <row r="13" spans="1:12" ht="61.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>64</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>11</v>
@@ -2317,7 +2344,7 @@
         <v>37</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
@@ -2333,7 +2360,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>11</v>
@@ -2345,7 +2372,7 @@
         <v>37</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
@@ -2361,7 +2388,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>11</v>
@@ -2373,7 +2400,7 @@
         <v>37</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -2389,7 +2416,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>11</v>
@@ -2401,7 +2428,7 @@
         <v>37</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
@@ -2515,7 +2542,7 @@
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>65</v>
@@ -2555,7 +2582,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -2698,12 +2725,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="34.5703125" customWidth="1"/>
     <col min="5" max="6" width="19.42578125" customWidth="1"/>
@@ -2738,17 +2766,27 @@
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
+      <c r="C2" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2">
+        <v>30</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="G2" s="2" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -2757,16 +2795,26 @@
       <c r="L2" s="14"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="B3" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5">
+        <v>25</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>123</v>
+      </c>
       <c r="G3" s="5" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -2775,16 +2823,26 @@
       <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
+      <c r="A4" s="9" t="s">
+        <v>116</v>
+      </c>
       <c r="B4" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="9"/>
+      <c r="C4" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="10">
+        <v>25</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>123</v>
+      </c>
       <c r="G4" s="10" t="s">
-        <v>72</v>
+        <v>122</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
@@ -2938,7 +2996,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2980,10 +3038,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2" t="s">
@@ -3006,10 +3064,10 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="10" t="s">
@@ -3046,7 +3104,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>

</xml_diff>

<commit_message>
modification du dico de données
</commit_message>
<xml_diff>
--- a/textes/Dictionnaire_données.xlsx
+++ b/textes/Dictionnaire_données.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" activeTab="4"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UTILISATEURS" sheetId="1" r:id="rId1"/>
-    <sheet name="FILTRES VOYAGES" sheetId="2" r:id="rId2"/>
-    <sheet name="VOYAGES" sheetId="4" r:id="rId3"/>
-    <sheet name="AMIS" sheetId="3" r:id="rId4"/>
-    <sheet name="NOTIFICATIONS" sheetId="5" r:id="rId5"/>
-    <sheet name="SIGNALEMENTS" sheetId="10" r:id="rId6"/>
+    <sheet name="langues" sheetId="11" r:id="rId2"/>
+    <sheet name="FILTRES VOYAGES" sheetId="2" r:id="rId3"/>
+    <sheet name="VOYAGES" sheetId="4" r:id="rId4"/>
+    <sheet name="AMIS" sheetId="3" r:id="rId5"/>
+    <sheet name="NOTIFICATIONS" sheetId="5" r:id="rId6"/>
+    <sheet name="SIGNALEMENTS" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="147">
   <si>
     <t>CODE</t>
   </si>
@@ -119,15 +120,6 @@
   </si>
   <si>
     <t>OUI ou NON</t>
-  </si>
-  <si>
-    <t>mylène</t>
-  </si>
-  <si>
-    <t>romain</t>
-  </si>
-  <si>
-    <t>nath</t>
   </si>
   <si>
     <t>NULL</t>
@@ -196,9 +188,6 @@
     <t>8 caractères minimum, dont 1 majuscule, 1 minuscule et 1 chiffre</t>
   </si>
   <si>
-    <t>Plusieurs possibles</t>
-  </si>
-  <si>
     <t>Est relié à "voyages"</t>
   </si>
   <si>
@@ -328,9 +317,6 @@
     <t>USERFRIEND</t>
   </si>
   <si>
-    <t>yoan</t>
-  </si>
-  <si>
     <t>USERREPORT</t>
   </si>
   <si>
@@ -456,6 +442,109 @@
   </si>
   <si>
     <t>OUI</t>
+  </si>
+  <si>
+    <t>anglais</t>
+  </si>
+  <si>
+    <t>espagnol</t>
+  </si>
+  <si>
+    <t>francais</t>
+  </si>
+  <si>
+    <t>allemand</t>
+  </si>
+  <si>
+    <t>arabe</t>
+  </si>
+  <si>
+    <t>chinois</t>
+  </si>
+  <si>
+    <t>japonais</t>
+  </si>
+  <si>
+    <t>russe</t>
+  </si>
+  <si>
+    <t>italien</t>
+  </si>
+  <si>
+    <t>neerlandais</t>
+  </si>
+  <si>
+    <t>portuguais</t>
+  </si>
+  <si>
+    <t>turc</t>
+  </si>
+  <si>
+    <t>coreen</t>
+  </si>
+  <si>
+    <t>Plusieurs possibles (1 minimum) est relié à langues</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PRIMARY KEY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> / Les caractères spéciaux ne sont pas acceptés
+(hors lettres avec accents, ‘ç’, ‘-‘, ‘ ?’, ‘ !’ et ‘ :’)</t>
+    </r>
+  </si>
+  <si>
+    <t>LANGANG</t>
+  </si>
+  <si>
+    <t>LANGESP</t>
+  </si>
+  <si>
+    <t>LANGFRA</t>
+  </si>
+  <si>
+    <t>LANGALL</t>
+  </si>
+  <si>
+    <t>LANGARA</t>
+  </si>
+  <si>
+    <t>LANGCHI</t>
+  </si>
+  <si>
+    <t>LANGJAP</t>
+  </si>
+  <si>
+    <t>LANGRUS</t>
+  </si>
+  <si>
+    <t>LANGIT</t>
+  </si>
+  <si>
+    <t>LANGNEER</t>
+  </si>
+  <si>
+    <t>LANGPOR</t>
+  </si>
+  <si>
+    <t>LANGTUR</t>
+  </si>
+  <si>
+    <t>LANGCOOR</t>
   </si>
 </sst>
 </file>
@@ -499,7 +588,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -703,11 +792,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -791,6 +909,25 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1075,7 +1212,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,10 +1239,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G1" s="14"/>
       <c r="H1" s="14"/>
@@ -1118,14 +1255,14 @@
         <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>19</v>
@@ -1141,7 +1278,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>11</v>
@@ -1150,10 +1287,10 @@
         <v>20</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
@@ -1166,17 +1303,17 @@
         <v>22</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -1189,7 +1326,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>11</v>
@@ -1198,7 +1335,7 @@
         <v>50</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="14"/>
@@ -1212,7 +1349,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>11</v>
@@ -1221,7 +1358,7 @@
         <v>50</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="14"/>
@@ -1235,7 +1372,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>18</v>
@@ -1244,10 +1381,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -1260,7 +1397,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>11</v>
@@ -1269,7 +1406,7 @@
         <v>50</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="14"/>
@@ -1283,17 +1420,17 @@
         <v>27</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -1315,7 +1452,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>29</v>
@@ -1328,10 +1465,10 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>11</v>
@@ -1340,7 +1477,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>29</v>
@@ -1495,9 +1632,7 @@
       <c r="K22" s="14"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>30</v>
-      </c>
+      <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -1530,10 +1665,296 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1048576"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="61.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2">
+        <v>30</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="7">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="7">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5">
+        <v>30</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="7">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5">
+        <v>30</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="16">
+        <v>30</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="16">
+        <v>30</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="16">
+        <v>30</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" s="33"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="16">
+        <v>30</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" s="33"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="10">
+        <v>30</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" s="32"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="30"/>
+    </row>
+    <row r="1048576" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1048576" s="31"/>
+      <c r="C1048576" s="35"/>
+      <c r="D1048576" s="31"/>
+      <c r="E1048576" s="35"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,10 +1984,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
@@ -1591,10 +2012,10 @@
         <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -1619,10 +2040,10 @@
         <v>60</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -1647,10 +2068,10 @@
         <v>60</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
@@ -1660,23 +2081,23 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>73</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>77</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -1686,23 +2107,23 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>78</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
@@ -1981,12 +2402,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2017,10 +2438,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
@@ -2028,15 +2449,15 @@
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
     </row>
-    <row r="2" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
@@ -2045,10 +2466,10 @@
         <v>50</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -2058,25 +2479,25 @@
     </row>
     <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="5">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -2086,13 +2507,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>18</v>
@@ -2101,10 +2522,10 @@
         <v>8</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
@@ -2114,13 +2535,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>18</v>
@@ -2129,10 +2550,10 @@
         <v>8</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -2142,20 +2563,20 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="14"/>
@@ -2166,20 +2587,20 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="14"/>
@@ -2190,13 +2611,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>11</v>
@@ -2205,10 +2626,10 @@
         <v>6</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -2218,22 +2639,22 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E9" s="5">
         <v>12</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>37</v>
+        <v>118</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="14"/>
@@ -2244,22 +2665,22 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E10" s="7">
         <v>12</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>37</v>
+        <v>118</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="14"/>
@@ -2270,13 +2691,13 @@
     </row>
     <row r="11" spans="1:12" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>11</v>
@@ -2285,10 +2706,10 @@
         <v>500</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>37</v>
+        <v>118</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
@@ -2298,13 +2719,13 @@
     </row>
     <row r="12" spans="1:12" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>11</v>
@@ -2313,10 +2734,10 @@
         <v>40</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>37</v>
+        <v>118</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
@@ -2324,27 +2745,27 @@
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
     </row>
-    <row r="13" spans="1:12" ht="61.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>95</v>
+    <row r="13" spans="1:12" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>90</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="5">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>37</v>
+        <v>118</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
@@ -2353,14 +2774,14 @@
       <c r="L13" s="14"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="34" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>11</v>
@@ -2369,10 +2790,10 @@
         <v>20</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
@@ -2388,7 +2809,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>11</v>
@@ -2397,10 +2818,10 @@
         <v>60</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -2409,26 +2830,26 @@
       <c r="L15" s="14"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="24" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="20">
         <v>60</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>37</v>
+        <v>118</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
@@ -2451,9 +2872,7 @@
       <c r="L18" s="14"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="17" t="s">
-        <v>31</v>
-      </c>
+      <c r="B19" s="17"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
@@ -2494,12 +2913,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2529,10 +2948,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
@@ -2542,10 +2961,10 @@
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="22" t="s">
@@ -2555,10 +2974,10 @@
         <v>20</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>37</v>
+        <v>118</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -2581,9 +3000,6 @@
       <c r="L4" s="14"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>81</v>
-      </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
@@ -2591,276 +3007,6 @@
       <c r="L5" s="14"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-    </row>
-    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-    </row>
-    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-    </row>
-    <row r="19" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-    </row>
-    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-    </row>
-    <row r="21" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-    </row>
-    <row r="22" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-    </row>
-    <row r="23" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" customWidth="1"/>
-    <col min="5" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="43.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-    </row>
-    <row r="2" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2">
-        <v>30</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="5">
-        <v>25</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="10">
-        <v>25</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
@@ -2996,7 +3142,275 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="43.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2">
+        <v>50</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5">
+        <v>45</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="10">
+        <v>45</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+    </row>
+    <row r="17" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+    </row>
+    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+    </row>
+    <row r="19" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+    </row>
+    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+    </row>
+    <row r="21" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+    </row>
+    <row r="22" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+    </row>
+    <row r="23" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3025,10 +3439,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
@@ -3038,10 +3452,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2" t="s">
@@ -3051,10 +3465,10 @@
         <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -3064,10 +3478,10 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="10" t="s">
@@ -3077,10 +3491,10 @@
         <v>20</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -3103,9 +3517,6 @@
       <c r="L5" s="14"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>81</v>
-      </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>

</xml_diff>

<commit_message>
Mise à jour du dictionnaire des données
</commit_message>
<xml_diff>
--- a/textes/Dictionnaire_données.xlsx
+++ b/textes/Dictionnaire_données.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="COMMENTAIRES" sheetId="11" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="57">
   <si>
     <t>CODE</t>
   </si>
@@ -318,6 +318,15 @@
       </rPr>
       <t xml:space="preserve"> / Table Etapes</t>
     </r>
+  </si>
+  <si>
+    <t>CONTINENT</t>
+  </si>
+  <si>
+    <t>PAYS</t>
+  </si>
+  <si>
+    <t>VILLE</t>
   </si>
 </sst>
 </file>
@@ -599,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -697,6 +706,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -980,7 +992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1048567"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -2303,10 +2315,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2437,20 +2449,20 @@
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
@@ -2458,16 +2470,18 @@
       <c r="K6" s="13"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>48</v>
+      <c r="A7" s="36" t="s">
+        <v>54</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5">
         <v>20</v>
       </c>
-      <c r="D7" s="5"/>
       <c r="E7" s="6" t="s">
         <v>8</v>
       </c>
@@ -2479,22 +2493,22 @@
       <c r="K7" s="13"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="A8" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="7">
-        <v>6</v>
+      <c r="D8" s="5">
+        <v>50</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
@@ -2502,119 +2516,164 @@
       <c r="K8" s="13"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
+      <c r="A9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="5">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="D9" s="7">
+        <v>50</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="F9" s="7"/>
       <c r="G9" s="13"/>
-      <c r="H9" s="13" t="s">
-        <v>51</v>
-      </c>
+      <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>50</v>
+      <c r="A10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="7">
-        <v>12</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F10" s="5"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="5">
-        <v>11</v>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="7">
+        <v>6</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="F11" s="7"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="10" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="5">
+        <v>12</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="35" t="s">
-        <v>53</v>
-      </c>
+      <c r="F12" s="5"/>
       <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
+      <c r="H12" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="7">
+        <v>12</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="7"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="5">
+        <v>11</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="16"/>
+    <row r="15" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="10">
+        <v>11</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>53</v>
+      </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
@@ -2628,27 +2687,49 @@
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
     </row>
-    <row r="17" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
     </row>
-    <row r="18" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="16"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
     </row>
-    <row r="19" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
     </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modification du dictionnaire des données
</commit_message>
<xml_diff>
--- a/textes/Dictionnaire_données.xlsx
+++ b/textes/Dictionnaire_données.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="COMMENTAIRES" sheetId="11" r:id="rId1"/>
@@ -17,8 +17,9 @@
     <sheet name="LANGUES" sheetId="13" r:id="rId3"/>
     <sheet name="NOTIFICATIONS" sheetId="5" r:id="rId4"/>
     <sheet name="SIGNALEMENTS" sheetId="10" r:id="rId5"/>
-    <sheet name="UTILISATEURS" sheetId="1" r:id="rId6"/>
-    <sheet name="VOYAGES" sheetId="4" r:id="rId7"/>
+    <sheet name="UTILISATEUR" sheetId="1" r:id="rId6"/>
+    <sheet name="DEMANDE_AMI" sheetId="14" r:id="rId7"/>
+    <sheet name="VOYAGES" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="62">
   <si>
     <t>CODE</t>
   </si>
@@ -74,9 +75,6 @@
     <t>COMMENTAIRE</t>
   </si>
   <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -105,9 +103,6 @@
   </si>
   <si>
     <t>CODE_NOTIF</t>
-  </si>
-  <si>
-    <t>TYPE_NOTIF</t>
   </si>
   <si>
     <t>CODE_SIGNAL</t>
@@ -327,6 +322,81 @@
   </si>
   <si>
     <t>VILLE</t>
+  </si>
+  <si>
+    <t>LIKES_ETAPE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>FOREIGN KEY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> / Table Voyage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">FOREIGN KEY </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/ Table Commentaire</t>
+    </r>
+  </si>
+  <si>
+    <t>ID_AMI</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">FOREIGN KEY </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/ Table Utilisateur</t>
+    </r>
+  </si>
+  <si>
+    <t>ACCEPTE</t>
+  </si>
+  <si>
+    <t>"Y" ou "N"</t>
   </si>
 </sst>
 </file>
@@ -990,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1048567"/>
+  <dimension ref="A1:F1048566"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,7 +1112,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1063,52 +1133,34 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="10">
         <v>11</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="10">
-        <v>11</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-    </row>
-    <row r="1048567" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1048567" s="23"/>
-      <c r="C1048567" s="25"/>
-      <c r="D1048567" s="23"/>
-      <c r="E1048567" s="25"/>
+      <c r="E4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
+    </row>
+    <row r="1048566" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1048566" s="23"/>
+      <c r="C1048566" s="25"/>
+      <c r="D1048566" s="23"/>
+      <c r="E1048566" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1121,7 +1173,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,10 +1207,10 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>10</v>
@@ -1170,15 +1222,15 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
@@ -1193,10 +1245,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
@@ -1211,13 +1263,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
@@ -1227,10 +1279,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>10</v>
@@ -1260,7 +1312,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1307,10 +1359,10 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>10</v>
@@ -1322,15 +1374,15 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>4</v>
@@ -1350,16 +1402,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="43.5703125" customWidth="1"/>
@@ -1391,23 +1443,23 @@
       <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="29">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>30</v>
+      <c r="E2" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>28</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -1415,20 +1467,18 @@
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>25</v>
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="5">
-        <v>15</v>
-      </c>
-      <c r="E3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="31" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="5"/>
@@ -1438,35 +1488,75 @@
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="10"/>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5">
+        <v>11</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>30</v>
+      </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="10">
+        <v>11</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
@@ -1592,8 +1682,23 @@
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
     </row>
+    <row r="24" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+    </row>
+    <row r="25" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1602,7 +1707,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,10 +1745,10 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -1655,7 +1760,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -1680,7 +1785,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
@@ -1839,7 +1944,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,10 +1984,10 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>10</v>
@@ -1894,7 +1999,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -1904,10 +2009,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>4</v>
@@ -1927,10 +2032,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
@@ -1950,10 +2055,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>4</v>
@@ -1965,7 +2070,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -1975,10 +2080,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>4</v>
@@ -1998,20 +2103,20 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
@@ -2021,10 +2126,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>6</v>
@@ -2042,10 +2147,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>4</v>
@@ -2065,10 +2170,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>4</v>
@@ -2080,7 +2185,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
@@ -2090,10 +2195,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>4</v>
@@ -2105,7 +2210,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
@@ -2115,10 +2220,10 @@
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>10</v>
@@ -2130,7 +2235,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
@@ -2314,6 +2419,107 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="29">
+        <v>11</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="7">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
@@ -2358,10 +2564,10 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>10</v>
@@ -2373,7 +2579,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -2383,10 +2589,10 @@
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
@@ -2406,10 +2612,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>4</v>
@@ -2429,10 +2635,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>6</v>
@@ -2450,10 +2656,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>6</v>
@@ -2471,10 +2677,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>4</v>
@@ -2494,10 +2700,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>4</v>
@@ -2517,10 +2723,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>4</v>
@@ -2540,13 +2746,13 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
@@ -2561,10 +2767,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>4</v>
@@ -2584,10 +2790,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>10</v>
@@ -2601,7 +2807,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
@@ -2609,10 +2815,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>10</v>
@@ -2632,10 +2838,10 @@
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>10</v>
@@ -2647,7 +2853,7 @@
         <v>8</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
@@ -2657,10 +2863,10 @@
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>10</v>
@@ -2672,7 +2878,7 @@
         <v>8</v>
       </c>
       <c r="F15" s="35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>

</xml_diff>

<commit_message>
Mise à jour dictionnaire de données
</commit_message>
<xml_diff>
--- a/textes/Dictionnaire_données.xlsx
+++ b/textes/Dictionnaire_données.xlsx
@@ -9,17 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="COMMENTAIRES" sheetId="11" r:id="rId1"/>
     <sheet name="ETAPES" sheetId="12" r:id="rId2"/>
     <sheet name="LANGUES" sheetId="13" r:id="rId3"/>
     <sheet name="NOTIFICATIONS" sheetId="5" r:id="rId4"/>
-    <sheet name="SIGNALEMENTS" sheetId="10" r:id="rId5"/>
-    <sheet name="UTILISATEUR" sheetId="1" r:id="rId6"/>
-    <sheet name="DEMANDE_AMI" sheetId="14" r:id="rId7"/>
-    <sheet name="VOYAGES" sheetId="4" r:id="rId8"/>
+    <sheet name="UTILISATEUR" sheetId="1" r:id="rId5"/>
+    <sheet name="DEMANDE_AMI" sheetId="14" r:id="rId6"/>
+    <sheet name="VOYAGES" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="60">
   <si>
     <t>CODE</t>
   </si>
@@ -100,9 +99,6 @@
   </si>
   <si>
     <t>CODE_NOTIF</t>
-  </si>
-  <si>
-    <t>CODE_SIGNAL</t>
   </si>
   <si>
     <t>PSEUDO</t>
@@ -150,27 +146,6 @@
         <family val="2"/>
       </rPr>
       <t>/ Auto_incrément</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>FOREIGN KEY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> / Table Commentaires</t>
     </r>
   </si>
   <si>
@@ -1178,7 +1153,7 @@
         <v>8</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1228,7 +1203,7 @@
         <v>8</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1257,7 +1232,7 @@
         <v>8</v>
       </c>
       <c r="I5" s="37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1329,7 +1304,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1427,7 +1402,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1512,7 +1487,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -1558,7 +1533,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
@@ -1568,10 +1543,10 @@
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>10</v>
@@ -1583,7 +1558,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -1608,7 +1583,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
@@ -1757,246 +1732,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="45.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-    </row>
-    <row r="3" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="10">
-        <v>11</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-    </row>
-    <row r="17" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-    </row>
-    <row r="18" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-    </row>
-    <row r="19" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-    </row>
-    <row r="20" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-    </row>
-    <row r="21" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-    </row>
-    <row r="22" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-    </row>
-    <row r="23" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -2052,7 +1790,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -2062,10 +1800,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>4</v>
@@ -2085,10 +1823,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
@@ -2108,10 +1846,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>4</v>
@@ -2123,7 +1861,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -2156,10 +1894,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>18</v>
@@ -2169,7 +1907,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
@@ -2179,10 +1917,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>6</v>
@@ -2200,10 +1938,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>4</v>
@@ -2223,10 +1961,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>4</v>
@@ -2238,7 +1976,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
@@ -2248,10 +1986,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>4</v>
@@ -2263,7 +2001,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
@@ -2288,7 +2026,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
@@ -2471,7 +2209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -2509,10 +2247,10 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>10</v>
@@ -2524,15 +2262,15 @@
         <v>8</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="30" t="s">
         <v>10</v>
@@ -2544,7 +2282,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2564,15 +2302,15 @@
         <v>8</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>4</v>
@@ -2584,7 +2322,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2592,11 +2330,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -2637,10 +2375,10 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>10</v>
@@ -2652,7 +2390,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -2662,10 +2400,10 @@
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
@@ -2685,10 +2423,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>4</v>
@@ -2708,10 +2446,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>6</v>
@@ -2729,10 +2467,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>6</v>
@@ -2750,10 +2488,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>4</v>
@@ -2773,10 +2511,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>4</v>
@@ -2796,10 +2534,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>4</v>
@@ -2819,10 +2557,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>18</v>
@@ -2840,10 +2578,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>4</v>
@@ -2880,7 +2618,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
@@ -2888,10 +2626,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>10</v>
@@ -2926,7 +2664,7 @@
         <v>8</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
@@ -2951,7 +2689,7 @@
         <v>8</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>

</xml_diff>

<commit_message>
Mise à jour du MCD et du dico des données
</commit_message>
<xml_diff>
--- a/textes/Dictionnaire_données.xlsx
+++ b/textes/Dictionnaire_données.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="COMMENTAIRES" sheetId="11" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="59">
   <si>
     <t>CODE</t>
   </si>
@@ -294,27 +294,6 @@
   </si>
   <si>
     <t>VILLE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>FOREIGN KEY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> / Table Voyage</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1232,7 +1211,7 @@
         <v>8</v>
       </c>
       <c r="I5" s="37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1430,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,23 +1520,23 @@
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="7" t="s">
+    <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="10">
         <v>11</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="E5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>52</v>
       </c>
       <c r="G5" s="13"/>
@@ -1566,25 +1545,7 @@
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="10">
-        <v>11</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>53</v>
-      </c>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
@@ -1716,13 +1677,6 @@
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
-    </row>
-    <row r="25" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1734,7 +1688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -2247,10 +2201,10 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>10</v>
@@ -2267,10 +2221,10 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="30" t="s">
         <v>10</v>
@@ -2282,7 +2236,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2302,15 +2256,15 @@
         <v>8</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>4</v>
@@ -2322,7 +2276,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>